<commit_message>
AA pathways over 50% and added SynPath code
</commit_message>
<xml_diff>
--- a/TransportDB/transportDB predictions.xlsx
+++ b/TransportDB/transportDB predictions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="328">
   <si>
     <t>ORF</t>
   </si>
@@ -937,13 +937,76 @@
   </si>
   <si>
     <t>ferrous ion</t>
+  </si>
+  <si>
+    <t>Associated w/NH3 transport in model</t>
+  </si>
+  <si>
+    <t>Not associated with any reactions in model</t>
+  </si>
+  <si>
+    <t>Associated w/Mg and Co transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Na and Ala transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Na and Pro transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Na and H+ transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/K transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Cyt. Transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Uracil transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Hypoxanthine transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Formate transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Sulfate transport in model</t>
+  </si>
+  <si>
+    <t>Assicuated w/Na Phosphate transport in model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Associated w/ Eha/Ehb in model </t>
+  </si>
+  <si>
+    <t>Associated w/Thiamin ABC Transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Betaine and Proline transporters in model</t>
+  </si>
+  <si>
+    <t>Associated w/Phosphate transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Glutamine transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Na-dependent ATP synthase</t>
+  </si>
+  <si>
+    <t>Associated w/Cu transport in model</t>
+  </si>
+  <si>
+    <t>Associated w/Fe transport in model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,6 +1024,12 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
     </font>
@@ -991,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1000,6 +1069,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,7 +1378,7 @@
   <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,6 +1386,7 @@
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="36.140625" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
@@ -1364,7 +1437,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1383,10 +1456,12 @@
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1405,7 +1480,9 @@
       <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1427,7 +1504,9 @@
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="4" t="s">
+        <v>308</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1449,7 +1528,9 @@
       <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="4" t="s">
+        <v>308</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1474,7 +1555,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1493,10 +1574,12 @@
       <c r="F8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>309</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1515,7 +1598,9 @@
       <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>309</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1720,7 +1805,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1739,10 +1824,12 @@
       <c r="F19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>311</v>
+      </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1761,10 +1848,12 @@
       <c r="F20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>311</v>
+      </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
@@ -1783,7 +1872,9 @@
       <c r="F21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>311</v>
+      </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1827,7 +1918,9 @@
       <c r="F23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>310</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>74</v>
       </c>
@@ -1876,7 +1969,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -1895,7 +1988,9 @@
       <c r="F26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1917,7 +2012,9 @@
       <c r="F27" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -1983,7 +2080,9 @@
       <c r="F30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2005,10 +2104,12 @@
       <c r="F31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>102</v>
       </c>
@@ -2027,7 +2128,9 @@
       <c r="F32" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2049,10 +2152,12 @@
       <c r="F33" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>314</v>
+      </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
@@ -2093,7 +2198,9 @@
       <c r="F35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2115,10 +2222,12 @@
       <c r="F36" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="4" t="s">
+        <v>316</v>
+      </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
@@ -2137,10 +2246,12 @@
       <c r="F37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>317</v>
+      </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -2162,7 +2273,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>133</v>
       </c>
@@ -2181,10 +2292,12 @@
       <c r="F39" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>138</v>
       </c>
@@ -2203,10 +2316,12 @@
       <c r="F40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>139</v>
       </c>
@@ -2225,7 +2340,9 @@
       <c r="F41" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>319</v>
+      </c>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2313,7 +2430,9 @@
       <c r="F45" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G45" s="2"/>
+      <c r="G45" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2335,7 +2454,9 @@
       <c r="F46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="2"/>
+      <c r="G46" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2357,7 +2478,9 @@
       <c r="F47" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="2"/>
+      <c r="G47" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -2379,8 +2502,8 @@
       <c r="F48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>45</v>
+      <c r="G48" s="4" t="s">
+        <v>320</v>
       </c>
       <c r="H48" s="2"/>
     </row>
@@ -2516,7 +2639,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>170</v>
       </c>
@@ -2648,7 +2771,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>192</v>
       </c>
@@ -2670,7 +2793,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>198</v>
       </c>
@@ -2692,7 +2815,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>199</v>
       </c>
@@ -2711,10 +2834,12 @@
       <c r="F63" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G63" s="2"/>
+      <c r="G63" s="4" t="s">
+        <v>321</v>
+      </c>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>200</v>
       </c>
@@ -2736,7 +2861,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>202</v>
       </c>
@@ -2758,7 +2883,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>203</v>
       </c>
@@ -2780,7 +2905,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>204</v>
       </c>
@@ -2802,7 +2927,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>205</v>
       </c>
@@ -2824,7 +2949,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>206</v>
       </c>
@@ -2846,7 +2971,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>207</v>
       </c>
@@ -2868,7 +2993,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>209</v>
       </c>
@@ -2890,7 +3015,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>210</v>
       </c>
@@ -2912,7 +3037,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>211</v>
       </c>
@@ -2934,7 +3059,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>212</v>
       </c>
@@ -2956,7 +3081,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>214</v>
       </c>
@@ -2978,7 +3103,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>215</v>
       </c>
@@ -3000,7 +3125,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>217</v>
       </c>
@@ -3022,7 +3147,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>219</v>
       </c>
@@ -3044,7 +3169,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>220</v>
       </c>
@@ -3066,7 +3191,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>221</v>
       </c>
@@ -3088,7 +3213,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>222</v>
       </c>
@@ -3110,7 +3235,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>223</v>
       </c>
@@ -3132,7 +3257,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>224</v>
       </c>
@@ -3154,7 +3279,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>225</v>
       </c>
@@ -3176,7 +3301,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>226</v>
       </c>
@@ -3198,7 +3323,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>227</v>
       </c>
@@ -3220,7 +3345,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>228</v>
       </c>
@@ -3242,7 +3367,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>229</v>
       </c>
@@ -3266,7 +3391,7 @@
       </c>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>231</v>
       </c>
@@ -3288,7 +3413,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>232</v>
       </c>
@@ -3310,7 +3435,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>233</v>
       </c>
@@ -3329,10 +3454,12 @@
       <c r="F91" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="G91" s="2"/>
+      <c r="G91" s="2" t="s">
+        <v>322</v>
+      </c>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>235</v>
       </c>
@@ -3354,7 +3481,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>236</v>
       </c>
@@ -3373,10 +3500,12 @@
       <c r="F93" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="G93" s="2"/>
+      <c r="G93" s="2" t="s">
+        <v>322</v>
+      </c>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>237</v>
       </c>
@@ -3398,7 +3527,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>238</v>
       </c>
@@ -3422,7 +3551,7 @@
       </c>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>240</v>
       </c>
@@ -3444,7 +3573,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>241</v>
       </c>
@@ -3463,10 +3592,12 @@
       <c r="F97" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G97" s="2"/>
+      <c r="G97" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>243</v>
       </c>
@@ -3485,10 +3616,12 @@
       <c r="F98" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G98" s="2"/>
+      <c r="G98" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>244</v>
       </c>
@@ -3507,10 +3640,12 @@
       <c r="F99" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G99" s="2"/>
+      <c r="G99" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>245</v>
       </c>
@@ -3529,10 +3664,12 @@
       <c r="F100" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G100" s="2"/>
+      <c r="G100" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>246</v>
       </c>
@@ -3551,10 +3688,12 @@
       <c r="F101" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G101" s="2"/>
+      <c r="G101" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>247</v>
       </c>
@@ -3576,7 +3715,7 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
     </row>
-    <row r="103" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>249</v>
       </c>
@@ -3598,7 +3737,7 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
     </row>
-    <row r="104" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>250</v>
       </c>
@@ -3620,7 +3759,7 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
     </row>
-    <row r="105" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>251</v>
       </c>
@@ -3642,7 +3781,7 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>252</v>
       </c>
@@ -3664,7 +3803,7 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>253</v>
       </c>
@@ -3686,7 +3825,7 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>254</v>
       </c>
@@ -3708,7 +3847,7 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
-    <row r="109" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>255</v>
       </c>
@@ -3730,7 +3869,7 @@
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
     </row>
-    <row r="110" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>256</v>
       </c>
@@ -3752,7 +3891,7 @@
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
     </row>
-    <row r="111" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>258</v>
       </c>
@@ -3774,7 +3913,7 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>259</v>
       </c>
@@ -3796,7 +3935,7 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
     </row>
-    <row r="113" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>260</v>
       </c>
@@ -3818,7 +3957,7 @@
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>261</v>
       </c>
@@ -3837,10 +3976,12 @@
       <c r="F114" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G114" s="2"/>
+      <c r="G114" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="H114" s="2"/>
     </row>
-    <row r="115" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>262</v>
       </c>
@@ -3862,7 +4003,7 @@
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
     </row>
-    <row r="116" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>263</v>
       </c>
@@ -3884,7 +4025,7 @@
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
     </row>
-    <row r="117" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>264</v>
       </c>
@@ -3906,7 +4047,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
     </row>
-    <row r="118" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>265</v>
       </c>
@@ -3928,7 +4069,7 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>267</v>
       </c>
@@ -3947,10 +4088,12 @@
       <c r="F119" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G119" s="2"/>
+      <c r="G119" s="4" t="s">
+        <v>321</v>
+      </c>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>268</v>
       </c>
@@ -3972,7 +4115,7 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>269</v>
       </c>
@@ -3994,7 +4137,7 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
     </row>
-    <row r="122" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>270</v>
       </c>
@@ -4013,12 +4156,10 @@
       <c r="F122" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G122" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="G122" s="2"/>
       <c r="H122" s="2"/>
     </row>
-    <row r="123" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>271</v>
       </c>
@@ -4040,7 +4181,7 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
     </row>
-    <row r="124" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>272</v>
       </c>
@@ -4081,7 +4222,9 @@
       <c r="F125" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G125" s="2"/>
+      <c r="G125" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H125" s="2"/>
     </row>
     <row r="126" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4103,7 +4246,9 @@
       <c r="F126" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G126" s="2"/>
+      <c r="G126" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H126" s="2"/>
     </row>
     <row r="127" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4125,7 +4270,9 @@
       <c r="F127" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G127" s="2"/>
+      <c r="G127" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H127" s="2"/>
     </row>
     <row r="128" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4147,7 +4294,9 @@
       <c r="F128" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G128" s="2"/>
+      <c r="G128" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H128" s="2"/>
     </row>
     <row r="129" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4169,7 +4318,9 @@
       <c r="F129" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G129" s="2"/>
+      <c r="G129" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H129" s="2"/>
     </row>
     <row r="130" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4191,7 +4342,9 @@
       <c r="F130" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G130" s="2"/>
+      <c r="G130" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H130" s="2"/>
     </row>
     <row r="131" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4213,7 +4366,9 @@
       <c r="F131" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G131" s="2"/>
+      <c r="G131" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H131" s="2"/>
     </row>
     <row r="132" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -4235,10 +4390,12 @@
       <c r="F132" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G132" s="2"/>
+      <c r="G132" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="H132" s="2"/>
     </row>
-    <row r="133" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>285</v>
       </c>
@@ -4260,7 +4417,7 @@
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
     </row>
-    <row r="134" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>290</v>
       </c>
@@ -4282,7 +4439,7 @@
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
     </row>
-    <row r="135" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>292</v>
       </c>
@@ -4304,7 +4461,7 @@
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
     </row>
-    <row r="136" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>293</v>
       </c>
@@ -4323,10 +4480,12 @@
       <c r="F136" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="G136" s="2"/>
+      <c r="G136" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="H136" s="2"/>
     </row>
-    <row r="137" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>295</v>
       </c>
@@ -4348,7 +4507,7 @@
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
     </row>
-    <row r="138" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>296</v>
       </c>
@@ -4388,6 +4547,9 @@
       </c>
       <c r="F139" s="2" t="s">
         <v>306</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heme and transporter updates
</commit_message>
<xml_diff>
--- a/TransportDB/transportDB predictions.xlsx
+++ b/TransportDB/transportDB predictions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="15576" windowHeight="9816"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1044,6 +1044,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,7 +1066,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1074,6 +1080,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1378,14 +1388,14 @@
   <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="36.109375" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1437,7 +1447,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1461,7 +1471,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1555,7 +1565,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1579,7 +1589,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1625,143 +1635,143 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="E12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="E14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="E16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -1783,7 +1793,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1805,7 +1815,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1829,7 +1839,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1853,7 +1863,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
@@ -1877,7 +1887,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
@@ -1899,7 +1909,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>69</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -1947,7 +1957,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -1969,7 +1979,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -1993,7 +2003,7 @@
       </c>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
@@ -2017,7 +2027,7 @@
       </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>94</v>
       </c>
@@ -2039,7 +2049,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>98</v>
       </c>
@@ -2061,7 +2071,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>100</v>
       </c>
@@ -2085,7 +2095,7 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>101</v>
       </c>
@@ -2109,7 +2119,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>102</v>
       </c>
@@ -2133,7 +2143,7 @@
       </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>107</v>
       </c>
@@ -2157,7 +2167,7 @@
       </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
@@ -2179,7 +2189,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>117</v>
       </c>
@@ -2203,7 +2213,7 @@
       </c>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>122</v>
       </c>
@@ -2227,7 +2237,7 @@
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
@@ -2251,7 +2261,7 @@
       </c>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -2273,7 +2283,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>133</v>
       </c>
@@ -2297,7 +2307,7 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>138</v>
       </c>
@@ -2321,7 +2331,7 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>139</v>
       </c>
@@ -2345,7 +2355,7 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>144</v>
       </c>
@@ -2367,7 +2377,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>149</v>
       </c>
@@ -2389,7 +2399,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>150</v>
       </c>
@@ -2411,7 +2421,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>152</v>
       </c>
@@ -2435,7 +2445,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>156</v>
       </c>
@@ -2459,7 +2469,7 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>157</v>
       </c>
@@ -2483,7 +2493,7 @@
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>158</v>
       </c>
@@ -2507,7 +2517,7 @@
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>159</v>
       </c>
@@ -2529,7 +2539,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>163</v>
       </c>
@@ -2551,7 +2561,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>165</v>
       </c>
@@ -2573,7 +2583,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>166</v>
       </c>
@@ -2595,7 +2605,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>167</v>
       </c>
@@ -2617,7 +2627,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>169</v>
       </c>
@@ -2639,7 +2649,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>170</v>
       </c>
@@ -2661,73 +2671,73 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="E56" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F57" s="2" t="s">
+      <c r="E57" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="E58" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>182</v>
       </c>
@@ -2749,7 +2759,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>187</v>
       </c>
@@ -2771,7 +2781,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>192</v>
       </c>
@@ -2793,7 +2803,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>198</v>
       </c>
@@ -2815,7 +2825,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>199</v>
       </c>
@@ -2839,7 +2849,7 @@
       </c>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>200</v>
       </c>
@@ -2861,7 +2871,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>202</v>
       </c>
@@ -2883,29 +2893,29 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="B66" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F66" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>204</v>
       </c>
@@ -2927,7 +2937,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>205</v>
       </c>
@@ -2949,7 +2959,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>206</v>
       </c>
@@ -2971,7 +2981,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>207</v>
       </c>
@@ -2993,7 +3003,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>209</v>
       </c>
@@ -3015,7 +3025,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>210</v>
       </c>
@@ -3037,7 +3047,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>211</v>
       </c>
@@ -3059,7 +3069,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>212</v>
       </c>
@@ -3081,7 +3091,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>214</v>
       </c>
@@ -3103,7 +3113,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>215</v>
       </c>
@@ -3125,7 +3135,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>217</v>
       </c>
@@ -3147,7 +3157,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>219</v>
       </c>
@@ -3169,7 +3179,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>220</v>
       </c>
@@ -3191,7 +3201,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>221</v>
       </c>
@@ -3213,7 +3223,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>222</v>
       </c>
@@ -3235,51 +3245,51 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="82" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="B82" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F82" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F83" s="2" t="s">
+      <c r="B83" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>225</v>
       </c>
@@ -3301,7 +3311,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>226</v>
       </c>
@@ -3323,7 +3333,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>227</v>
       </c>
@@ -3345,7 +3355,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>228</v>
       </c>
@@ -3367,7 +3377,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>229</v>
       </c>
@@ -3391,51 +3401,51 @@
       </c>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="89" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F89" s="2" t="s">
+      <c r="B89" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F90" s="2" t="s">
+      <c r="B90" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>233</v>
       </c>
@@ -3459,7 +3469,7 @@
       </c>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>235</v>
       </c>
@@ -3481,7 +3491,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>236</v>
       </c>
@@ -3505,29 +3515,29 @@
       </c>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+    <row r="94" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F94" s="2" t="s">
+      <c r="B94" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F94" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>238</v>
       </c>
@@ -3551,7 +3561,7 @@
       </c>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>240</v>
       </c>
@@ -3573,7 +3583,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>241</v>
       </c>
@@ -3597,7 +3607,7 @@
       </c>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>243</v>
       </c>
@@ -3621,7 +3631,7 @@
       </c>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>244</v>
       </c>
@@ -3645,7 +3655,7 @@
       </c>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>245</v>
       </c>
@@ -3669,7 +3679,7 @@
       </c>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>246</v>
       </c>
@@ -3693,7 +3703,7 @@
       </c>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>247</v>
       </c>
@@ -3715,7 +3725,7 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>249</v>
       </c>
@@ -3737,7 +3747,7 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>250</v>
       </c>
@@ -3759,7 +3769,7 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>251</v>
       </c>
@@ -3781,7 +3791,7 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>252</v>
       </c>
@@ -3803,7 +3813,7 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>253</v>
       </c>
@@ -3825,7 +3835,7 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>254</v>
       </c>
@@ -3847,7 +3857,7 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>255</v>
       </c>
@@ -3869,7 +3879,7 @@
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>256</v>
       </c>
@@ -3891,7 +3901,7 @@
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>258</v>
       </c>
@@ -3913,7 +3923,7 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>259</v>
       </c>
@@ -3935,7 +3945,7 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>260</v>
       </c>
@@ -3957,7 +3967,7 @@
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>261</v>
       </c>
@@ -3981,7 +3991,7 @@
       </c>
       <c r="H114" s="2"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>262</v>
       </c>
@@ -4003,7 +4013,7 @@
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>263</v>
       </c>
@@ -4025,7 +4035,7 @@
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>264</v>
       </c>
@@ -4047,7 +4057,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>265</v>
       </c>
@@ -4069,7 +4079,7 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>267</v>
       </c>
@@ -4093,7 +4103,7 @@
       </c>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>268</v>
       </c>
@@ -4115,7 +4125,7 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>269</v>
       </c>
@@ -4137,7 +4147,7 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>270</v>
       </c>
@@ -4159,7 +4169,7 @@
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>271</v>
       </c>
@@ -4181,7 +4191,7 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>272</v>
       </c>
@@ -4203,7 +4213,7 @@
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
     </row>
-    <row r="125" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>273</v>
       </c>
@@ -4227,7 +4237,7 @@
       </c>
       <c r="H125" s="2"/>
     </row>
-    <row r="126" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>278</v>
       </c>
@@ -4251,7 +4261,7 @@
       </c>
       <c r="H126" s="2"/>
     </row>
-    <row r="127" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>279</v>
       </c>
@@ -4275,7 +4285,7 @@
       </c>
       <c r="H127" s="2"/>
     </row>
-    <row r="128" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>280</v>
       </c>
@@ -4299,7 +4309,7 @@
       </c>
       <c r="H128" s="2"/>
     </row>
-    <row r="129" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>281</v>
       </c>
@@ -4323,7 +4333,7 @@
       </c>
       <c r="H129" s="2"/>
     </row>
-    <row r="130" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>282</v>
       </c>
@@ -4347,7 +4357,7 @@
       </c>
       <c r="H130" s="2"/>
     </row>
-    <row r="131" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>283</v>
       </c>
@@ -4371,7 +4381,7 @@
       </c>
       <c r="H131" s="2"/>
     </row>
-    <row r="132" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>284</v>
       </c>
@@ -4395,29 +4405,29 @@
       </c>
       <c r="H132" s="2"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+    <row r="133" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D133" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="E133" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F133" s="2" t="s">
+      <c r="E133" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F133" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G133" s="5"/>
+      <c r="H133" s="5"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>290</v>
       </c>
@@ -4439,7 +4449,7 @@
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>292</v>
       </c>
@@ -4461,7 +4471,7 @@
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>293</v>
       </c>
@@ -4485,7 +4495,7 @@
       </c>
       <c r="H136" s="2"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>295</v>
       </c>
@@ -4507,7 +4517,7 @@
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>296</v>
       </c>
@@ -4529,7 +4539,7 @@
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>301</v>
       </c>
@@ -4564,7 +4574,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4576,7 +4586,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added acetamido sugars, AA syn, transporters, etc
</commit_message>
<xml_diff>
--- a/TransportDB/transportDB predictions.xlsx
+++ b/TransportDB/transportDB predictions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="15576" windowHeight="9816"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="15570" windowHeight="9810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1075,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1098,6 +1098,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1403,15 +1406,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1463,7 +1466,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1487,7 +1490,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1511,77 +1514,77 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1605,7 +1608,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1629,7 +1632,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1651,7 +1654,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -1765,7 +1768,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
@@ -1787,7 +1790,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -1809,7 +1812,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1831,7 +1834,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1855,7 +1858,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1879,7 +1882,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
@@ -1903,7 +1906,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
@@ -1925,7 +1928,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="7" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>69</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -1995,7 +1998,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -2019,7 +2022,7 @@
       </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="7" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
@@ -2043,7 +2046,7 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>94</v>
       </c>
@@ -2065,7 +2068,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="7" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>98</v>
       </c>
@@ -2087,7 +2090,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="7" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>100</v>
       </c>
@@ -2111,7 +2114,7 @@
       </c>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="7" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>101</v>
       </c>
@@ -2135,7 +2138,7 @@
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>102</v>
       </c>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>107</v>
       </c>
@@ -2183,7 +2186,7 @@
       </c>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
@@ -2205,7 +2208,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>117</v>
       </c>
@@ -2229,7 +2232,7 @@
       </c>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>122</v>
       </c>
@@ -2253,7 +2256,7 @@
       </c>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>123</v>
       </c>
@@ -2277,7 +2280,7 @@
       </c>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -2299,7 +2302,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>133</v>
       </c>
@@ -2323,7 +2326,7 @@
       </c>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>138</v>
       </c>
@@ -2347,7 +2350,7 @@
       </c>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>139</v>
       </c>
@@ -2371,169 +2374,169 @@
       </c>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="2" t="s">
+      <c r="E42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="E43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="E44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="E45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G45" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F46" s="2" t="s">
+      <c r="E46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="E47" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="E48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G48" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" s="6" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>159</v>
       </c>
@@ -2555,7 +2558,7 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>163</v>
       </c>
@@ -2577,7 +2580,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" s="6" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>165</v>
       </c>
@@ -2599,7 +2602,7 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8" s="6" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>166</v>
       </c>
@@ -2621,7 +2624,7 @@
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="1:8" s="6" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>167</v>
       </c>
@@ -2643,7 +2646,7 @@
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8" s="6" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="6" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>169</v>
       </c>
@@ -2665,7 +2668,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>170</v>
       </c>
@@ -2687,7 +2690,7 @@
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>175</v>
       </c>
@@ -2709,7 +2712,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>180</v>
       </c>
@@ -2731,7 +2734,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>181</v>
       </c>
@@ -2753,51 +2756,51 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F59" s="2" t="s">
+      <c r="E59" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="2" t="s">
+      <c r="E60" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>192</v>
       </c>
@@ -2819,7 +2822,7 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>198</v>
       </c>
@@ -2841,7 +2844,7 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>199</v>
       </c>
@@ -2865,7 +2868,7 @@
       </c>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>200</v>
       </c>
@@ -2887,7 +2890,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>202</v>
       </c>
@@ -2909,7 +2912,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>203</v>
       </c>
@@ -2931,7 +2934,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>204</v>
       </c>
@@ -2953,7 +2956,7 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>205</v>
       </c>
@@ -2975,7 +2978,7 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>206</v>
       </c>
@@ -2997,7 +3000,7 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>207</v>
       </c>
@@ -3019,7 +3022,7 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>209</v>
       </c>
@@ -3041,7 +3044,7 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>210</v>
       </c>
@@ -3063,7 +3066,7 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>211</v>
       </c>
@@ -3085,51 +3088,51 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F74" s="2" t="s">
+      <c r="B74" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F75" s="2" t="s">
+      <c r="B75" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>215</v>
       </c>
@@ -3151,7 +3154,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>217</v>
       </c>
@@ -3173,7 +3176,7 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>219</v>
       </c>
@@ -3195,7 +3198,7 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>220</v>
       </c>
@@ -3217,7 +3220,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>221</v>
       </c>
@@ -3239,7 +3242,7 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>222</v>
       </c>
@@ -3261,7 +3264,7 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>223</v>
       </c>
@@ -3283,7 +3286,7 @@
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
     </row>
-    <row r="83" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>224</v>
       </c>
@@ -3305,119 +3308,119 @@
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="B84" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F84" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F85" s="2" t="s">
+      <c r="B85" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F85" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F86" s="2" t="s">
+      <c r="B86" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F86" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F87" s="2" t="s">
+      <c r="B87" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F88" s="2" t="s">
+      <c r="B88" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H88" s="2"/>
-    </row>
-    <row r="89" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>231</v>
       </c>
@@ -3439,7 +3442,7 @@
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
     </row>
-    <row r="90" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>232</v>
       </c>
@@ -3461,7 +3464,7 @@
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>233</v>
       </c>
@@ -3485,7 +3488,7 @@
       </c>
       <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>235</v>
       </c>
@@ -3507,7 +3510,7 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>236</v>
       </c>
@@ -3531,7 +3534,7 @@
       </c>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>237</v>
       </c>
@@ -3553,53 +3556,53 @@
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+    <row r="95" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F95" s="2" t="s">
+      <c r="B95" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G95" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H95" s="2"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F96" s="2" t="s">
+      <c r="B96" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>241</v>
       </c>
@@ -3623,7 +3626,7 @@
       </c>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>243</v>
       </c>
@@ -3647,7 +3650,7 @@
       </c>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>244</v>
       </c>
@@ -3671,7 +3674,7 @@
       </c>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>245</v>
       </c>
@@ -3695,7 +3698,7 @@
       </c>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>246</v>
       </c>
@@ -3719,51 +3722,51 @@
       </c>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F102" s="2" t="s">
+      <c r="B102" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F102" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F103" s="2" t="s">
+      <c r="B103" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>250</v>
       </c>
@@ -3785,7 +3788,7 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>251</v>
       </c>
@@ -3807,7 +3810,7 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>252</v>
       </c>
@@ -3829,7 +3832,7 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>253</v>
       </c>
@@ -3851,7 +3854,7 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>254</v>
       </c>
@@ -3873,7 +3876,7 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>255</v>
       </c>
@@ -3895,95 +3898,95 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F110" s="2" t="s">
+      <c r="B110" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F111" s="2" t="s">
+      <c r="B111" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F111" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F112" s="2" t="s">
+      <c r="B112" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F112" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+    </row>
+    <row r="113" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F113" s="2" t="s">
+      <c r="B113" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F113" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+    </row>
+    <row r="114" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>261</v>
       </c>
@@ -4007,73 +4010,73 @@
       </c>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
+    <row r="115" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F115" s="2" t="s">
+      <c r="B115" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F116" s="2" t="s">
+      <c r="B116" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F116" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F117" s="2" t="s">
+      <c r="B117" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>265</v>
       </c>
@@ -4095,7 +4098,7 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>267</v>
       </c>
@@ -4119,7 +4122,7 @@
       </c>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>268</v>
       </c>
@@ -4141,7 +4144,7 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>269</v>
       </c>
@@ -4163,7 +4166,7 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
     </row>
-    <row r="122" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>270</v>
       </c>
@@ -4185,7 +4188,7 @@
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>271</v>
       </c>
@@ -4207,7 +4210,7 @@
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>272</v>
       </c>
@@ -4229,7 +4232,7 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>273</v>
       </c>
@@ -4253,7 +4256,7 @@
       </c>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>278</v>
       </c>
@@ -4277,7 +4280,7 @@
       </c>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>279</v>
       </c>
@@ -4301,7 +4304,7 @@
       </c>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>280</v>
       </c>
@@ -4325,7 +4328,7 @@
       </c>
       <c r="H128" s="3"/>
     </row>
-    <row r="129" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>281</v>
       </c>
@@ -4349,7 +4352,7 @@
       </c>
       <c r="H129" s="3"/>
     </row>
-    <row r="130" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>282</v>
       </c>
@@ -4373,7 +4376,7 @@
       </c>
       <c r="H130" s="3"/>
     </row>
-    <row r="131" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>283</v>
       </c>
@@ -4397,7 +4400,7 @@
       </c>
       <c r="H131" s="3"/>
     </row>
-    <row r="132" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>284</v>
       </c>
@@ -4421,7 +4424,7 @@
       </c>
       <c r="H132" s="3"/>
     </row>
-    <row r="133" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>285</v>
       </c>
@@ -4443,51 +4446,51 @@
       <c r="G133" s="5"/>
       <c r="H133" s="5"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
+    <row r="134" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="D134" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="E134" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F134" s="2" t="s">
+      <c r="E134" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F134" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+    </row>
+    <row r="135" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="D135" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="E135" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F135" s="2" t="s">
+      <c r="E135" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F135" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-    </row>
-    <row r="136" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+    </row>
+    <row r="136" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>293</v>
       </c>
@@ -4511,7 +4514,7 @@
       </c>
       <c r="H136" s="3"/>
     </row>
-    <row r="137" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>295</v>
       </c>
@@ -4533,29 +4536,29 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
+    <row r="138" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="D138" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="E138" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F138" s="2" t="s">
+      <c r="E138" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F138" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-    </row>
-    <row r="139" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>301</v>
       </c>
@@ -4590,7 +4593,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4602,7 +4605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>